<commit_message>
fixes to decision tree and random forest
</commit_message>
<xml_diff>
--- a/tickerdata_day_returns.xlsx
+++ b/tickerdata_day_returns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anand\Documents\CS229\project\wsb-stock-prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DA4B64-52FF-4441-AF57-70481B3E8C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF31516-9054-4E9A-B6BE-C231F46E8596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -123,7 +123,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,16 +141,28 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF232A31"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -186,11 +198,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -204,6 +225,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -509,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z140"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -518,7 +543,7 @@
     <col min="1" max="1" width="18.109375" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -602,80 +627,80 @@
       <c r="A2" s="5">
         <v>44223</v>
       </c>
-      <c r="B2">
-        <v>39.540000915527337</v>
-      </c>
-      <c r="C2">
-        <v>20.412616839381361</v>
+      <c r="B2" s="6">
+        <v>32.97</v>
+      </c>
+      <c r="C2" s="6">
+        <v>23.73</v>
       </c>
       <c r="D2">
         <v>3.8499999046325679</v>
       </c>
-      <c r="E2">
-        <v>11.97999954223633</v>
-      </c>
-      <c r="F2">
-        <v>23.29999923706055</v>
-      </c>
-      <c r="G2">
-        <v>46.509998321533203</v>
-      </c>
-      <c r="H2">
-        <v>89.830001831054688</v>
-      </c>
-      <c r="I2">
-        <v>76.67247687000912</v>
-      </c>
-      <c r="J2">
-        <v>265</v>
-      </c>
-      <c r="K2">
-        <v>820</v>
-      </c>
-      <c r="L2">
-        <v>42</v>
-      </c>
-      <c r="M2">
-        <v>461.57998657226563</v>
-      </c>
-      <c r="N2">
-        <v>19.469999313354489</v>
-      </c>
-      <c r="O2">
-        <v>14.77999973297119</v>
-      </c>
-      <c r="P2">
-        <v>5.1584164145277542</v>
-      </c>
-      <c r="Q2">
-        <v>7.1900009562062923</v>
-      </c>
-      <c r="R2">
-        <v>30.120000839233398</v>
-      </c>
-      <c r="S2">
-        <v>9.4243105227563735</v>
-      </c>
-      <c r="T2">
-        <v>14.71903684936227</v>
+      <c r="E2" s="6">
+        <v>20.34</v>
+      </c>
+      <c r="F2" s="6">
+        <v>23.35</v>
+      </c>
+      <c r="G2" s="6">
+        <v>44.66</v>
+      </c>
+      <c r="H2" s="6">
+        <v>91.1</v>
+      </c>
+      <c r="I2" s="6">
+        <v>78.34</v>
+      </c>
+      <c r="J2" s="6">
+        <v>354.83</v>
+      </c>
+      <c r="K2" s="6">
+        <v>870.35</v>
+      </c>
+      <c r="L2" s="6">
+        <v>37.17</v>
+      </c>
+      <c r="M2" s="6">
+        <v>478.84</v>
+      </c>
+      <c r="N2" s="6">
+        <v>20.25</v>
+      </c>
+      <c r="O2" s="6">
+        <v>15.4</v>
+      </c>
+      <c r="P2" s="6">
+        <v>4.99</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="R2" s="7">
+        <v>26.49</v>
+      </c>
+      <c r="S2" s="6">
+        <v>9.43</v>
+      </c>
+      <c r="T2" s="6">
+        <v>15.28</v>
       </c>
       <c r="U2">
         <v>7.9099998474121094</v>
       </c>
-      <c r="V2">
-        <v>56.759998321533203</v>
+      <c r="V2" s="6">
+        <v>57.95</v>
       </c>
       <c r="W2">
         <v>1</v>
       </c>
-      <c r="X2">
-        <v>0.95800000429153442</v>
-      </c>
-      <c r="Y2">
-        <v>20.329999923706051</v>
-      </c>
-      <c r="Z2">
-        <v>54.496894517965259</v>
+      <c r="X2" s="6">
+        <v>0.505</v>
+      </c>
+      <c r="Y2" s="6">
+        <v>15.42</v>
+      </c>
+      <c r="Z2" s="6">
+        <v>57.3</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.3">
@@ -11720,7 +11745,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -11733,8 +11758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5B32C54-5754-4E5C-BEE3-846ADB864041}">
   <dimension ref="A1:Z139"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11828,11 +11853,11 @@
       </c>
       <c r="B2">
         <f>(Sheet1!B3-Sheet1!B2)/Sheet1!B2</f>
-        <v>0</v>
+        <v>0.19927209328260048</v>
       </c>
       <c r="C2">
         <f>(Sheet1!C3-Sheet1!C2)/Sheet1!C2</f>
-        <v>0</v>
+        <v>-0.13979701477533246</v>
       </c>
       <c r="D2">
         <f>(Sheet1!D3-Sheet1!D2)/Sheet1!D2</f>
@@ -11840,67 +11865,67 @@
       </c>
       <c r="E2">
         <f>(Sheet1!E3-Sheet1!E2)/Sheet1!E2</f>
-        <v>0</v>
+        <v>-0.41101280519978711</v>
       </c>
       <c r="F2">
         <f>(Sheet1!F3-Sheet1!F2)/Sheet1!F2</f>
-        <v>0</v>
+        <v>-2.1413602971927619E-3</v>
       </c>
       <c r="G2">
         <f>(Sheet1!G3-Sheet1!G2)/Sheet1!G2</f>
-        <v>0</v>
+        <v>4.1424055565006869E-2</v>
       </c>
       <c r="H2">
         <f>(Sheet1!H3-Sheet1!H2)/Sheet1!H2</f>
-        <v>0</v>
+        <v>-1.3940704379202052E-2</v>
       </c>
       <c r="I2">
         <f>(Sheet1!I3-Sheet1!I2)/Sheet1!I2</f>
-        <v>0</v>
+        <v>-2.1285717768584157E-2</v>
       </c>
       <c r="J2">
         <f>(Sheet1!J3-Sheet1!J2)/Sheet1!J2</f>
-        <v>0</v>
+        <v>-0.25316348674012906</v>
       </c>
       <c r="K2">
         <f>(Sheet1!K3-Sheet1!K2)/Sheet1!K2</f>
-        <v>0</v>
+        <v>-5.7850290113172886E-2</v>
       </c>
       <c r="L2">
         <f>(Sheet1!L3-Sheet1!L2)/Sheet1!L2</f>
-        <v>0</v>
+        <v>0.1299435028248587</v>
       </c>
       <c r="M2">
         <f>(Sheet1!M3-Sheet1!M2)/Sheet1!M2</f>
-        <v>0</v>
+        <v>-3.6045471196504787E-2</v>
       </c>
       <c r="N2">
         <f>(Sheet1!N3-Sheet1!N2)/Sheet1!N2</f>
-        <v>0</v>
+        <v>-3.8518552426938836E-2</v>
       </c>
       <c r="O2">
         <f>(Sheet1!O3-Sheet1!O2)/Sheet1!O2</f>
-        <v>0</v>
+        <v>-4.0259757599273423E-2</v>
       </c>
       <c r="P2">
         <f>(Sheet1!P3-Sheet1!P2)/Sheet1!P2</f>
-        <v>0</v>
+        <v>3.37507844744998E-2</v>
       </c>
       <c r="Q2">
         <f>(Sheet1!Q3-Sheet1!Q2)/Sheet1!Q2</f>
-        <v>0</v>
+        <v>-0.13373482455345884</v>
       </c>
       <c r="R2">
         <f>(Sheet1!R3-Sheet1!R2)/Sheet1!R2</f>
-        <v>0</v>
+        <v>0.13703287426324651</v>
       </c>
       <c r="S2">
         <f>(Sheet1!S3-Sheet1!S2)/Sheet1!S2</f>
-        <v>0</v>
+        <v>-6.0333798978008787E-4</v>
       </c>
       <c r="T2">
         <f>(Sheet1!T3-Sheet1!T2)/Sheet1!T2</f>
-        <v>0</v>
+        <v>-3.6712248078385412E-2</v>
       </c>
       <c r="U2">
         <f>(Sheet1!U3-Sheet1!U2)/Sheet1!U2</f>
@@ -11908,7 +11933,7 @@
       </c>
       <c r="V2">
         <f>(Sheet1!V3-Sheet1!V2)/Sheet1!V2</f>
-        <v>0</v>
+        <v>-2.0534972881221737E-2</v>
       </c>
       <c r="W2">
         <f>(Sheet1!W3-Sheet1!W2)/Sheet1!W2</f>
@@ -11916,15 +11941,15 @@
       </c>
       <c r="X2">
         <f>(Sheet1!X3-Sheet1!X2)/Sheet1!X2</f>
-        <v>0</v>
+        <v>0.89702971146838495</v>
       </c>
       <c r="Y2">
         <f>(Sheet1!Y3-Sheet1!Y2)/Sheet1!Y2</f>
-        <v>0</v>
+        <v>0.31841763448158567</v>
       </c>
       <c r="Z2">
         <f>(Sheet1!Z3-Sheet1!Z2)/Sheet1!Z2</f>
-        <v>0</v>
+        <v>-4.8919816440396821E-2</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.3">

</xml_diff>